<commit_message>
Catch up updates on excel sheets
</commit_message>
<xml_diff>
--- a/ContentBudget.xlsx
+++ b/ContentBudget.xlsx
@@ -1,43 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanks\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33C255B-7BFF-42E0-B6D6-A67D7C064B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{B9D99D12-1771-499A-AABF-A52B4DF2B140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{01F8A032-1727-4E1F-B7EF-1F1B723FD455}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01F8A032-1727-4E1F-B7EF-1F1B723FD455}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>Wurrzug</t>
   </si>
@@ -154,6 +147,105 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Demonettes</t>
+  </si>
+  <si>
+    <t>Steeds of Excess</t>
+  </si>
+  <si>
+    <t>Chariots of Excess</t>
+  </si>
+  <si>
+    <t>Keepers of The Forbidden</t>
+  </si>
+  <si>
+    <t>N'Kari</t>
+  </si>
+  <si>
+    <t>Two New Spells of Excess</t>
+  </si>
+  <si>
+    <t>Fiends of Excess</t>
+  </si>
+  <si>
+    <t>Magic Items of Escess</t>
+  </si>
+  <si>
+    <t>Thricefold Discord</t>
+  </si>
+  <si>
+    <t>Warrior Priests</t>
+  </si>
+  <si>
+    <t>Witch Hunters</t>
+  </si>
+  <si>
+    <t>Falgellants + RoR</t>
+  </si>
+  <si>
+    <t>War Altar</t>
+  </si>
+  <si>
+    <t>Volkmar The Grim</t>
+  </si>
+  <si>
+    <t>Luthor Huss</t>
+  </si>
+  <si>
+    <t>Sacred Magic Items</t>
+  </si>
+  <si>
+    <t>Mace of Helsturm</t>
+  </si>
+  <si>
+    <t>White Cloak of Ulric</t>
+  </si>
+  <si>
+    <t>Sword of Rightious Steel</t>
+  </si>
+  <si>
+    <t>Hammer of Judgement</t>
+  </si>
+  <si>
+    <t>Jade Amulet</t>
+  </si>
+  <si>
+    <t>Rod of Command</t>
+  </si>
+  <si>
+    <t>Icon of Magnus</t>
+  </si>
+  <si>
+    <t>4 Witchhunters</t>
+  </si>
+  <si>
+    <t>Holy Warriors</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Settra</t>
+  </si>
+  <si>
+    <t>Nekaph</t>
+  </si>
+  <si>
+    <t>Khalida</t>
+  </si>
+  <si>
+    <t>Apophas</t>
+  </si>
+  <si>
+    <t>Arkhan</t>
+  </si>
+  <si>
+    <t>Khemric Titan</t>
+  </si>
+  <si>
+    <t>Bone Dragon</t>
   </si>
 </sst>
 </file>
@@ -201,18 +293,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -233,9 +325,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -273,7 +365,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -379,7 +471,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -521,13 +613,844 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EE2407-AD4D-4545-9973-352764C32E26}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.6328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="21.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.90625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="14.26953125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="2">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
+        <f>SUM(B2:E2)</f>
+        <v>23</v>
+      </c>
+      <c r="G2" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="2">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F12" si="0">SUM(B3:E3)</f>
+        <v>15</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="2">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="2">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
+        <v>34</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2">
+        <f>SUM(F2:F12)</f>
+        <v>118</v>
+      </c>
+      <c r="G13" s="2">
+        <f>SUM(G2:G12)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="F16" s="2">
+        <f>SUM(B16:E16)</f>
+        <v>15</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="2">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2">
+        <f>SUM(B17:E17)</f>
+        <v>15</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="2">
+        <v>15</v>
+      </c>
+      <c r="F18" s="2">
+        <f>SUM(B18:E18)</f>
+        <v>15</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F19" s="2">
+        <f>SUM(B19:E19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F20" s="2">
+        <f>SUM(B20:E20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="2">
+        <f>SUM(F16:F20)</f>
+        <v>45</v>
+      </c>
+      <c r="G21" s="2">
+        <f>SUM(G16:G20)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="2">
+        <f>F13+F21</f>
+        <v>163</v>
+      </c>
+      <c r="G22" s="2">
+        <f>G13+G21</f>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G2:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28521718-FE0E-48B4-B149-9563C56013BE}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="20.6328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="21.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.90625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16.1796875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="14.26953125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="2">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2">
+        <f>SUM(B2:E2)</f>
+        <v>14</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F12" si="0">SUM(B3:E3)</f>
+        <v>18</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="2">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="2">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="2">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2">
+        <f>SUM(F2:F12)</f>
+        <v>96</v>
+      </c>
+      <c r="G13" s="2">
+        <f>SUM(G2:G12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="F16" s="2">
+        <f>SUM(B16:E16)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="2">
+        <v>24</v>
+      </c>
+      <c r="F17" s="2">
+        <f>SUM(B17:E17)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="2">
+        <f>SUM(B18:E18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="2">
+        <f>SUM(B19:E19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="2">
+        <f>SUM(B20:E20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="2">
+        <f>SUM(F16:F20)</f>
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108676E2-ECB3-4528-BC41-A72A153FEED1}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="29.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="2">
+        <v>26</v>
+      </c>
+      <c r="F2" s="2">
+        <f>SUM(B2:E2)</f>
+        <v>26</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="2">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F13" si="0">SUM(B4:E4)</f>
+        <v>13</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2">
+        <f>SUM(F2:F13)</f>
+        <v>93</v>
+      </c>
+      <c r="G14" s="2">
+        <f>SUM(G2:G13)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2">
+        <v>45</v>
+      </c>
+      <c r="F17" s="2">
+        <f>SUM(B17:E17)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="2">
+        <f>SUM(B18:E18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="2">
+        <f>SUM(B19:E19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="2">
+        <f>SUM(B20:E20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F21" s="2">
+        <f>SUM(B21:E21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="2">
+        <f>SUM(F17:F21)</f>
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D43BCB-7D99-47FD-92B3-939E705405EA}">
   <dimension ref="A1:G23"/>
   <sheetViews>
@@ -599,7 +1522,7 @@
         <f t="shared" ref="F3:F12" si="0">SUM(B3:E3)</f>
         <v>5</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="5">
         <v>2</v>
       </c>
     </row>
@@ -614,7 +1537,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -627,7 +1550,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -640,7 +1563,7 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="5">
         <v>2</v>
       </c>
     </row>
@@ -655,7 +1578,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -668,7 +1591,7 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -771,7 +1694,7 @@
         <v>5</v>
       </c>
       <c r="F17">
-        <f t="shared" ref="F17:F20" si="1">SUM(B17:E17)</f>
+        <f>SUM(B17:E17)</f>
         <v>5</v>
       </c>
     </row>
@@ -783,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="F18">
-        <f t="shared" si="1"/>
+        <f>SUM(B18:E18)</f>
         <v>5</v>
       </c>
     </row>
@@ -795,7 +1718,7 @@
         <v>15</v>
       </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f>SUM(B19:E19)</f>
         <v>15</v>
       </c>
     </row>
@@ -816,7 +1739,7 @@
         <v>4</v>
       </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f>SUM(B20:E20)</f>
         <v>23</v>
       </c>
     </row>
@@ -849,276 +1772,276 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1595F44-BF1C-410F-B7E6-FA1156A41470}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.36328125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="5"/>
+    <col min="1" max="1" width="29.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="5">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5">
+      <c r="B2" s="2">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2">
         <f>SUM(B2:E2)</f>
         <v>15</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="2">
         <v>8</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="2">
         <f t="shared" ref="F3:F12" si="0">SUM(B3:E3)</f>
         <v>8</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <v>8</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="5">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="B5" s="2">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G5" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="2">
         <v>8</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="5">
-        <v>15</v>
-      </c>
-      <c r="C7" s="5">
-        <v>2</v>
-      </c>
-      <c r="D7" s="5">
-        <v>2</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="B7" s="2">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
         <v>4</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="B8" s="2">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="2">
         <v>10</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F10" s="5">
+      <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F11" s="5">
+      <c r="F11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F12" s="5">
+      <c r="F12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="2">
         <f>SUM(F2:F12)</f>
         <v>104</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="2">
         <f>SUM(G2:G12)</f>
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5">
-        <v>15</v>
-      </c>
-      <c r="C16" s="5">
-        <v>2</v>
-      </c>
-      <c r="D16" s="5">
-        <v>2</v>
-      </c>
-      <c r="E16" s="5">
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2">
         <v>4</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="2">
         <f>SUM(B16:E16)</f>
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="5">
-        <v>15</v>
-      </c>
-      <c r="F17" s="5">
-        <f t="shared" ref="F17:F20" si="1">SUM(B17:E17)</f>
+      <c r="B17" s="2">
+        <v>15</v>
+      </c>
+      <c r="F17" s="2">
+        <f>SUM(B17:E17)</f>
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="2">
         <v>16</v>
       </c>
-      <c r="F18" s="5">
-        <f t="shared" si="1"/>
+      <c r="F18" s="2">
+        <f>SUM(B18:E18)</f>
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F19" s="5">
-        <f t="shared" si="1"/>
+      <c r="F19" s="2">
+        <f>SUM(B19:E19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F20" s="5">
-        <f t="shared" si="1"/>
+      <c r="F20" s="2">
+        <f>SUM(B20:E20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="2">
         <f>SUM(F16:F20)</f>
         <v>54</v>
       </c>

</xml_diff>